<commit_message>
Manual user testing/ burndown chart
</commit_message>
<xml_diff>
--- a/Misc. Files/Manual User Testing/Manual user Testing.xlsx
+++ b/Misc. Files/Manual User Testing/Manual user Testing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack McMahon\Documents\QUT\IT\YEar 2\IFB299\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack\Documents\QUT Sem 2\IAB299\ifb299_Team12\Misc. Files\Manual User Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BFE63E3-0849-4792-9E6E-CFE596DFD42D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C578255-2680-4443-A8A7-FC16F90D7B49}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" firstSheet="5" activeTab="7" xr2:uid="{ED100DB8-B1E1-4BE5-B5E1-D95E4BDE2B1A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" firstSheet="2" activeTab="7" xr2:uid="{ED100DB8-B1E1-4BE5-B5E1-D95E4BDE2B1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual User testing" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="388">
   <si>
     <t>Project name</t>
   </si>
@@ -1555,7 +1555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1646,6 +1646,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1964,28 +1968,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{948BE22D-8575-4D6C-AB16-B1A1D96443BC}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="84" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="59" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="10" style="12" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.26171875" customWidth="1"/>
+    <col min="3" max="3" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83984375" customWidth="1"/>
+    <col min="5" max="5" width="13.41796875" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83984375" customWidth="1"/>
+    <col min="8" max="8" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="15.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -1993,7 +1997,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
@@ -2004,7 +2008,7 @@
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
     </row>
-    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
@@ -2012,7 +2016,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
@@ -2020,19 +2024,19 @@
         <v>43372</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="20"/>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="20"/>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="21"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="18" t="s">
         <v>16</v>
       </c>
@@ -2076,7 +2080,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="22" t="s">
         <v>34</v>
       </c>
@@ -2112,7 +2116,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="7"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2142,7 +2146,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="115.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11" s="7"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2172,7 +2176,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="115.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
         <v>35</v>
@@ -2206,7 +2210,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="7"/>
       <c r="D13" s="2" t="s">
         <v>64</v>
@@ -2234,7 +2238,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="7"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2264,7 +2268,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2294,7 +2298,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="7"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2310,7 +2314,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="7"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2326,7 +2330,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="7"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2342,7 +2346,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A19" s="7"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2358,7 +2362,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:14" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="158.69999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A20" s="7"/>
       <c r="B20" s="2" t="s">
         <v>38</v>
@@ -2394,7 +2398,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="255" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="7"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2426,7 +2430,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="7"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2442,7 +2446,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="7"/>
       <c r="B23" s="10" t="s">
         <v>40</v>
@@ -2478,7 +2482,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="7"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -2494,7 +2498,7 @@
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
     </row>
-    <row r="25" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="7"/>
       <c r="B25" s="10" t="s">
         <v>42</v>
@@ -2516,7 +2520,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="7"/>
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
@@ -2532,7 +2536,7 @@
       <c r="M26" s="10"/>
       <c r="N26" s="11"/>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A27" s="7"/>
       <c r="B27" s="10"/>
       <c r="C27" s="11"/>
@@ -2548,7 +2552,7 @@
       <c r="M27" s="10"/>
       <c r="N27" s="11"/>
     </row>
-    <row r="28" spans="1:14" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="57.9" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A28" s="22" t="s">
         <v>17</v>
       </c>
@@ -2570,7 +2574,7 @@
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
     </row>
-    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A29" s="7"/>
       <c r="B29" s="13"/>
       <c r="C29" s="7"/>
@@ -2586,7 +2590,7 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
     </row>
-    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A30" s="7"/>
       <c r="B30" s="13"/>
       <c r="C30" s="7"/>
@@ -2602,7 +2606,7 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
     </row>
-    <row r="31" spans="1:14" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="86.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A31" s="7"/>
       <c r="B31" s="13" t="s">
         <v>82</v>
@@ -2622,7 +2626,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
     </row>
-    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A32" s="7"/>
       <c r="B32" s="13"/>
       <c r="C32" s="7"/>
@@ -2638,7 +2642,7 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
     </row>
-    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A33" s="7"/>
       <c r="B33" s="13" t="s">
         <v>83</v>
@@ -2656,7 +2660,7 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A34" s="7"/>
       <c r="B34" s="13"/>
       <c r="C34" s="7"/>
@@ -2672,7 +2676,7 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
     </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A35" s="7"/>
       <c r="B35" s="13" t="s">
         <v>84</v>
@@ -2690,7 +2694,7 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A36" s="7"/>
       <c r="B36" s="13"/>
       <c r="C36" s="7"/>
@@ -2706,7 +2710,7 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
     </row>
-    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A37" s="7"/>
       <c r="B37" s="13" t="s">
         <v>85</v>
@@ -2724,7 +2728,7 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="7"/>
       <c r="B38" s="2"/>
       <c r="C38" s="7"/>
@@ -2754,20 +2758,20 @@
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83984375" customWidth="1"/>
+    <col min="4" max="4" width="14.41796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83984375" customWidth="1"/>
+    <col min="6" max="6" width="20.83984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.68359375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.15625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -2775,7 +2779,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
@@ -2786,7 +2790,7 @@
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
     </row>
-    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
@@ -2794,7 +2798,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
@@ -2802,19 +2806,19 @@
         <v>43367</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="20"/>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="20"/>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="21"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="18" t="s">
         <v>16</v>
       </c>
@@ -2858,7 +2862,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
         <v>89</v>
       </c>
@@ -2894,7 +2898,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2924,7 +2928,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2940,7 +2944,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>91</v>
@@ -2972,7 +2976,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2988,7 +2992,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -3004,7 +3008,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
         <v>92</v>
@@ -3038,7 +3042,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -3054,7 +3058,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -3070,7 +3074,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
         <v>93</v>
@@ -3104,7 +3108,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -3120,7 +3124,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -3136,7 +3140,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
         <v>94</v>
@@ -3170,7 +3174,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3196,7 +3200,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -3212,7 +3216,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2"/>
       <c r="B24" s="10" t="s">
         <v>81</v>
@@ -3246,7 +3250,7 @@
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3262,7 +3266,7 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -3278,7 +3282,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -3294,7 +3298,7 @@
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
     </row>
-    <row r="28" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
         <v>95</v>
@@ -3326,7 +3330,7 @@
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -3342,7 +3346,7 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -3358,7 +3362,7 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -3374,7 +3378,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -3390,7 +3394,7 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -3406,7 +3410,7 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -3422,7 +3426,7 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -3438,7 +3442,7 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -3454,7 +3458,7 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -3483,24 +3487,24 @@
       <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.68359375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.15625" customWidth="1"/>
+    <col min="7" max="7" width="19.578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.83984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.26171875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.83984375" customWidth="1"/>
+    <col min="12" max="12" width="12.41796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.15625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -3508,7 +3512,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
@@ -3517,7 +3521,7 @@
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
     </row>
-    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
@@ -3525,25 +3529,25 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="14"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="20"/>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="20"/>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="21"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="18" t="s">
         <v>16</v>
       </c>
@@ -3587,7 +3591,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
         <v>121</v>
       </c>
@@ -3623,7 +3627,7 @@
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
     </row>
-    <row r="10" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3653,7 +3657,7 @@
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3669,7 +3673,7 @@
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
     </row>
-    <row r="12" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>123</v>
@@ -3701,7 +3705,7 @@
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3717,7 +3721,7 @@
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -3733,7 +3737,7 @@
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -3749,7 +3753,7 @@
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -3765,7 +3769,7 @@
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
     </row>
-    <row r="17" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
         <v>124</v>
@@ -3799,7 +3803,7 @@
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3815,7 +3819,7 @@
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -3831,7 +3835,7 @@
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
     </row>
-    <row r="20" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
         <v>125</v>
@@ -3865,7 +3869,7 @@
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3881,7 +3885,7 @@
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3897,7 +3901,7 @@
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
     </row>
-    <row r="23" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
         <v>126</v>
@@ -3931,7 +3935,7 @@
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3947,7 +3951,7 @@
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3963,7 +3967,7 @@
       <c r="M25" s="7"/>
       <c r="N25" s="7"/>
     </row>
-    <row r="26" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
         <v>127</v>
@@ -3997,7 +4001,7 @@
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="7"/>
@@ -4013,7 +4017,7 @@
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -4029,7 +4033,7 @@
       <c r="M28" s="7"/>
       <c r="N28" s="7"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -4045,7 +4049,7 @@
       <c r="M29" s="7"/>
       <c r="N29" s="7"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -4061,7 +4065,7 @@
       <c r="M30" s="7"/>
       <c r="N30" s="7"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -4077,7 +4081,7 @@
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -4093,7 +4097,7 @@
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -4109,7 +4113,7 @@
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -4125,7 +4129,7 @@
       <c r="M34" s="7"/>
       <c r="N34" s="7"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -4141,7 +4145,7 @@
       <c r="M35" s="7"/>
       <c r="N35" s="7"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -4170,23 +4174,23 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.15625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.26171875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="13.41796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.15625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.41796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -4194,7 +4198,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
@@ -4203,7 +4207,7 @@
       <c r="D2" s="15"/>
       <c r="E2" s="32"/>
     </row>
-    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
@@ -4211,25 +4215,25 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="14"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="20"/>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="20"/>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="21"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="24" t="s">
         <v>16</v>
       </c>
@@ -4273,7 +4277,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
         <v>132</v>
       </c>
@@ -4299,7 +4303,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2"/>
       <c r="B10" s="27"/>
       <c r="C10" s="7"/>
@@ -4315,7 +4319,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2"/>
       <c r="B11" s="27"/>
       <c r="C11" s="7"/>
@@ -4331,7 +4335,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2"/>
       <c r="B12" s="27" t="s">
         <v>134</v>
@@ -4355,7 +4359,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2"/>
       <c r="B13" s="27"/>
       <c r="C13" s="2"/>
@@ -4375,7 +4379,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2"/>
       <c r="B14" s="27" t="s">
         <v>135</v>
@@ -4397,7 +4401,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2"/>
       <c r="B15" s="27"/>
       <c r="C15" s="2"/>
@@ -4413,7 +4417,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2"/>
       <c r="B16" s="27" t="s">
         <v>136</v>
@@ -4435,7 +4439,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2"/>
       <c r="B17" s="27"/>
       <c r="C17" s="7"/>
@@ -4451,7 +4455,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2"/>
       <c r="B18" s="27" t="s">
         <v>137</v>
@@ -4473,7 +4477,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2"/>
       <c r="B19" s="27"/>
       <c r="C19" s="2"/>
@@ -4489,7 +4493,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2"/>
       <c r="B20" s="27" t="s">
         <v>138</v>
@@ -4511,7 +4515,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2"/>
       <c r="B21" s="27"/>
       <c r="C21" s="29"/>
@@ -4527,7 +4531,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2"/>
       <c r="B22" s="27" t="s">
         <v>139</v>
@@ -4549,7 +4553,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2"/>
       <c r="B23" s="27"/>
       <c r="C23" s="7"/>
@@ -4565,7 +4569,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2"/>
       <c r="B24" s="27" t="s">
         <v>140</v>
@@ -4587,7 +4591,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2"/>
       <c r="B25" s="27"/>
       <c r="C25" s="7"/>
@@ -4603,7 +4607,7 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
     </row>
-    <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2"/>
       <c r="B26" s="27" t="s">
         <v>141</v>
@@ -4625,7 +4629,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="7"/>
@@ -4641,7 +4645,7 @@
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -4657,7 +4661,7 @@
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -4673,7 +4677,7 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="7"/>
@@ -4689,7 +4693,7 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -4705,7 +4709,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -4721,7 +4725,7 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="7"/>
@@ -4737,7 +4741,7 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -4753,7 +4757,7 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -4769,7 +4773,7 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="7"/>
@@ -4785,7 +4789,7 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="7"/>
@@ -4801,7 +4805,7 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -4817,7 +4821,7 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -4833,7 +4837,7 @@
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -4849,7 +4853,7 @@
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -4865,7 +4869,7 @@
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -4881,7 +4885,7 @@
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -4897,7 +4901,7 @@
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -4913,7 +4917,7 @@
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -4929,7 +4933,7 @@
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -4959,20 +4963,20 @@
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="8.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83984375" customWidth="1"/>
+    <col min="5" max="5" width="14.68359375" customWidth="1"/>
+    <col min="6" max="6" width="13.41796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.26171875" style="12" customWidth="1"/>
     <col min="8" max="8" width="15" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -4980,7 +4984,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
@@ -4989,7 +4993,7 @@
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
     </row>
-    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
@@ -4997,25 +5001,25 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="14"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="20"/>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="20"/>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="21"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="24" t="s">
         <v>16</v>
       </c>
@@ -5059,7 +5063,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="30" t="s">
         <v>151</v>
       </c>
@@ -5083,7 +5087,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="30"/>
       <c r="B10" s="27"/>
       <c r="C10" s="31"/>
@@ -5099,7 +5103,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="30"/>
       <c r="B11" s="27" t="s">
         <v>153</v>
@@ -5129,7 +5133,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="30"/>
       <c r="B12" s="27"/>
       <c r="C12" s="32"/>
@@ -5145,7 +5149,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="30"/>
       <c r="B13" s="27" t="s">
         <v>154</v>
@@ -5175,7 +5179,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="30"/>
       <c r="B14" s="27"/>
       <c r="C14" s="32"/>
@@ -5191,7 +5195,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="30"/>
       <c r="B15" s="27" t="s">
         <v>155</v>
@@ -5223,7 +5227,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="30"/>
       <c r="B16" s="27"/>
       <c r="C16" s="31"/>
@@ -5239,7 +5243,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="30"/>
       <c r="B17" s="27" t="s">
         <v>156</v>
@@ -5271,7 +5275,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="30"/>
       <c r="B18" s="27"/>
       <c r="C18" s="32"/>
@@ -5287,7 +5291,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="39"/>
       <c r="B19" s="40" t="s">
         <v>157</v>
@@ -5309,7 +5313,7 @@
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="30"/>
       <c r="B20" s="27"/>
       <c r="C20" s="31"/>
@@ -5325,7 +5329,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="39"/>
       <c r="B21" s="40" t="s">
         <v>158</v>
@@ -5347,7 +5351,7 @@
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="30"/>
       <c r="B22" s="27"/>
       <c r="C22" s="32"/>
@@ -5363,7 +5367,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="30"/>
       <c r="B23" s="27" t="s">
         <v>159</v>
@@ -5393,7 +5397,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="30"/>
       <c r="B24" s="27"/>
       <c r="C24" s="33"/>
@@ -5409,7 +5413,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="30"/>
       <c r="B25" s="27" t="s">
         <v>160</v>
@@ -5433,7 +5437,7 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="30"/>
       <c r="B26" s="27"/>
       <c r="C26" s="32"/>
@@ -5449,7 +5453,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
     </row>
-    <row r="27" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="30"/>
       <c r="B27" s="27" t="s">
         <v>161</v>
@@ -5477,7 +5481,7 @@
       <c r="M27" s="7"/>
       <c r="N27" s="2"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2"/>
       <c r="B28" s="34"/>
       <c r="C28" s="2"/>
@@ -5493,7 +5497,7 @@
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2"/>
       <c r="B29" s="26"/>
       <c r="C29" s="28"/>
@@ -5509,7 +5513,7 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2"/>
       <c r="B30" s="26"/>
       <c r="C30" s="29"/>
@@ -5525,7 +5529,7 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2"/>
       <c r="B31" s="26"/>
       <c r="C31" s="23"/>
@@ -5541,7 +5545,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2"/>
       <c r="B32" s="26"/>
       <c r="C32" s="7"/>
@@ -5557,7 +5561,7 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2"/>
       <c r="B33" s="26"/>
       <c r="C33" s="23"/>
@@ -5573,7 +5577,7 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2"/>
       <c r="B34" s="26"/>
       <c r="C34" s="7"/>
@@ -5589,7 +5593,7 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2"/>
       <c r="B35" s="26"/>
       <c r="C35" s="23"/>
@@ -5605,7 +5609,7 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="7"/>
@@ -5621,7 +5625,7 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -5637,7 +5641,7 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -5653,7 +5657,7 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="7"/>
@@ -5669,7 +5673,7 @@
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -5685,7 +5689,7 @@
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -5701,7 +5705,7 @@
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="7"/>
@@ -5717,7 +5721,7 @@
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -5733,7 +5737,7 @@
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -5749,7 +5753,7 @@
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="7"/>
@@ -5765,7 +5769,7 @@
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="7"/>
@@ -5781,7 +5785,7 @@
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -5797,7 +5801,7 @@
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -5813,7 +5817,7 @@
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -5829,7 +5833,7 @@
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -5845,7 +5849,7 @@
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -5861,7 +5865,7 @@
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -5877,7 +5881,7 @@
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -5893,7 +5897,7 @@
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -5909,7 +5913,7 @@
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -5934,22 +5938,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E828D426-AE19-4984-A91E-F96A4B3B1AB6}">
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="A9" zoomScale="54" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.15625" customWidth="1"/>
+    <col min="4" max="4" width="13.15625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83984375" customWidth="1"/>
+    <col min="6" max="6" width="13.41796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.26171875" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -5957,7 +5961,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
@@ -5966,7 +5970,7 @@
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
     </row>
-    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
@@ -5974,25 +5978,25 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="14"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="20"/>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="20"/>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="21"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="24" t="s">
         <v>16</v>
       </c>
@@ -6036,7 +6040,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="30" t="s">
         <v>177</v>
       </c>
@@ -6068,7 +6072,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="30"/>
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
@@ -6084,7 +6088,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="30"/>
       <c r="B11" s="27" t="s">
         <v>172</v>
@@ -6110,7 +6114,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="30"/>
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
@@ -6126,7 +6130,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="30"/>
       <c r="B13" s="27" t="s">
         <v>173</v>
@@ -6158,7 +6162,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="30"/>
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
@@ -6174,7 +6178,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="30"/>
       <c r="B15" s="27" t="s">
         <v>174</v>
@@ -6206,7 +6210,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="30"/>
       <c r="B16" s="27"/>
       <c r="C16" s="27"/>
@@ -6222,7 +6226,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="30"/>
       <c r="B17" s="27" t="s">
         <v>175</v>
@@ -6254,7 +6258,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="30"/>
       <c r="B18" s="27"/>
       <c r="C18" s="27"/>
@@ -6282,7 +6286,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="30"/>
       <c r="B19" s="27" t="s">
         <v>176</v>
@@ -6306,13 +6310,15 @@
         <v>338</v>
       </c>
       <c r="I19" s="2"/>
-      <c r="J19" s="10"/>
+      <c r="J19" s="42" t="s">
+        <v>258</v>
+      </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="30"/>
       <c r="B20" s="35"/>
       <c r="C20" s="23"/>
@@ -6328,7 +6334,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="30"/>
       <c r="B21" s="27"/>
       <c r="C21" s="31"/>
@@ -6344,7 +6350,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="30"/>
       <c r="B22" s="26"/>
       <c r="C22" s="23"/>
@@ -6360,7 +6366,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="30"/>
       <c r="B23" s="26"/>
       <c r="C23" s="32"/>
@@ -6376,7 +6382,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="30"/>
       <c r="B24" s="26"/>
       <c r="C24" s="23"/>
@@ -6392,7 +6398,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="30"/>
       <c r="B25" s="26"/>
       <c r="C25" s="31"/>
@@ -6408,7 +6414,7 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="30"/>
       <c r="B26" s="26"/>
       <c r="C26" s="23"/>
@@ -6424,7 +6430,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="30"/>
       <c r="B27" s="26"/>
       <c r="C27" s="32"/>
@@ -6440,7 +6446,7 @@
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="30"/>
       <c r="B28" s="26"/>
       <c r="C28" s="23"/>
@@ -6456,7 +6462,7 @@
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="30"/>
       <c r="B29" s="26"/>
       <c r="C29" s="33"/>
@@ -6472,7 +6478,7 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="30"/>
       <c r="B30" s="26"/>
       <c r="C30" s="23"/>
@@ -6488,7 +6494,7 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="30"/>
       <c r="B31" s="26"/>
       <c r="C31" s="32"/>
@@ -6504,7 +6510,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="30"/>
       <c r="B32" s="26"/>
       <c r="C32" s="23"/>
@@ -6520,7 +6526,7 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2"/>
       <c r="B33" s="34"/>
       <c r="C33" s="2"/>
@@ -6536,7 +6542,7 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2"/>
       <c r="B34" s="26"/>
       <c r="C34" s="28"/>
@@ -6552,7 +6558,7 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2"/>
       <c r="B35" s="26"/>
       <c r="C35" s="29"/>
@@ -6568,7 +6574,7 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2"/>
       <c r="B36" s="26"/>
       <c r="C36" s="23"/>
@@ -6584,7 +6590,7 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2"/>
       <c r="B37" s="26"/>
       <c r="C37" s="7"/>
@@ -6600,7 +6606,7 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2"/>
       <c r="B38" s="26"/>
       <c r="C38" s="23"/>
@@ -6616,7 +6622,7 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2"/>
       <c r="B39" s="26"/>
       <c r="C39" s="7"/>
@@ -6632,7 +6638,7 @@
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="2"/>
       <c r="B40" s="26"/>
       <c r="C40" s="23"/>
@@ -6648,7 +6654,7 @@
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="7"/>
@@ -6664,7 +6670,7 @@
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -6680,7 +6686,7 @@
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -6696,7 +6702,7 @@
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="7"/>
@@ -6712,7 +6718,7 @@
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -6728,7 +6734,7 @@
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -6744,7 +6750,7 @@
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="7"/>
@@ -6760,7 +6766,7 @@
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -6776,7 +6782,7 @@
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -6792,7 +6798,7 @@
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="7"/>
@@ -6808,7 +6814,7 @@
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="7"/>
@@ -6824,7 +6830,7 @@
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -6840,7 +6846,7 @@
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -6856,7 +6862,7 @@
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -6872,7 +6878,7 @@
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -6888,7 +6894,7 @@
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -6904,7 +6910,7 @@
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -6920,7 +6926,7 @@
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -6936,7 +6942,7 @@
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -6952,7 +6958,7 @@
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -6977,22 +6983,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E713E43-55FD-4508-932B-858E3BEA571A}">
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="A4" zoomScale="55" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.15625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.578125" customWidth="1"/>
+    <col min="6" max="6" width="13.41796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -7000,7 +7006,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
@@ -7009,7 +7015,7 @@
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
     </row>
-    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
@@ -7017,25 +7023,25 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="14"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="20"/>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="20"/>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="21"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="24" t="s">
         <v>16</v>
       </c>
@@ -7079,7 +7085,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="30" t="s">
         <v>182</v>
       </c>
@@ -7113,7 +7119,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="30"/>
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
@@ -7129,7 +7135,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="30"/>
       <c r="B11" s="27" t="s">
         <v>185</v>
@@ -7161,7 +7167,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="30"/>
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
@@ -7177,7 +7183,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="30"/>
       <c r="B13" s="27" t="s">
         <v>187</v>
@@ -7203,7 +7209,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="30"/>
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
@@ -7219,7 +7225,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="30"/>
       <c r="B15" s="27" t="s">
         <v>188</v>
@@ -7251,7 +7257,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="30"/>
       <c r="B16" s="27"/>
       <c r="C16" s="27"/>
@@ -7267,7 +7273,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="30"/>
       <c r="B17" s="27" t="s">
         <v>190</v>
@@ -7297,7 +7303,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="30"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
@@ -7313,7 +7319,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="30"/>
       <c r="B19" s="27"/>
       <c r="C19" s="27"/>
@@ -7329,7 +7335,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="30"/>
       <c r="B20" s="27"/>
       <c r="C20" s="27"/>
@@ -7345,7 +7351,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="30"/>
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
@@ -7361,7 +7367,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="30"/>
       <c r="B22" s="27"/>
       <c r="C22" s="27"/>
@@ -7377,7 +7383,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="30"/>
       <c r="B23" s="27"/>
       <c r="C23" s="27"/>
@@ -7393,7 +7399,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="30"/>
       <c r="B24" s="35"/>
       <c r="C24" s="23"/>
@@ -7409,7 +7415,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="30"/>
       <c r="B25" s="27"/>
       <c r="C25" s="31"/>
@@ -7425,7 +7431,7 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="30"/>
       <c r="B26" s="26"/>
       <c r="C26" s="23"/>
@@ -7441,7 +7447,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="30"/>
       <c r="B27" s="26"/>
       <c r="C27" s="32"/>
@@ -7457,7 +7463,7 @@
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="30"/>
       <c r="B28" s="26"/>
       <c r="C28" s="23"/>
@@ -7473,7 +7479,7 @@
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="30"/>
       <c r="B29" s="26"/>
       <c r="C29" s="31"/>
@@ -7489,7 +7495,7 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="30"/>
       <c r="B30" s="26"/>
       <c r="C30" s="23"/>
@@ -7505,7 +7511,7 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="30"/>
       <c r="B31" s="26"/>
       <c r="C31" s="32"/>
@@ -7521,7 +7527,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="30"/>
       <c r="B32" s="26"/>
       <c r="C32" s="23"/>
@@ -7537,7 +7543,7 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="30"/>
       <c r="B33" s="26"/>
       <c r="C33" s="33"/>
@@ -7553,7 +7559,7 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="30"/>
       <c r="B34" s="26"/>
       <c r="C34" s="23"/>
@@ -7569,7 +7575,7 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="30"/>
       <c r="B35" s="26"/>
       <c r="C35" s="32"/>
@@ -7585,7 +7591,7 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="30"/>
       <c r="B36" s="26"/>
       <c r="C36" s="23"/>
@@ -7601,7 +7607,7 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2"/>
       <c r="B37" s="34"/>
       <c r="C37" s="2"/>
@@ -7617,7 +7623,7 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2"/>
       <c r="B38" s="26"/>
       <c r="C38" s="28"/>
@@ -7633,7 +7639,7 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2"/>
       <c r="B39" s="26"/>
       <c r="C39" s="29"/>
@@ -7649,7 +7655,7 @@
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="2"/>
       <c r="B40" s="26"/>
       <c r="C40" s="23"/>
@@ -7665,7 +7671,7 @@
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2"/>
       <c r="B41" s="26"/>
       <c r="C41" s="7"/>
@@ -7681,7 +7687,7 @@
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2"/>
       <c r="B42" s="26"/>
       <c r="C42" s="23"/>
@@ -7697,7 +7703,7 @@
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2"/>
       <c r="B43" s="26"/>
       <c r="C43" s="7"/>
@@ -7713,7 +7719,7 @@
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2"/>
       <c r="B44" s="26"/>
       <c r="C44" s="23"/>
@@ -7729,7 +7735,7 @@
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="7"/>
@@ -7745,7 +7751,7 @@
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -7761,7 +7767,7 @@
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -7777,7 +7783,7 @@
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="7"/>
@@ -7793,7 +7799,7 @@
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -7809,7 +7815,7 @@
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -7825,7 +7831,7 @@
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="7"/>
@@ -7841,7 +7847,7 @@
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -7857,7 +7863,7 @@
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -7873,7 +7879,7 @@
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="7"/>
@@ -7889,7 +7895,7 @@
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="7"/>
@@ -7905,7 +7911,7 @@
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -7921,7 +7927,7 @@
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -7937,7 +7943,7 @@
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -7953,7 +7959,7 @@
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -7969,7 +7975,7 @@
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -7985,7 +7991,7 @@
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -8001,7 +8007,7 @@
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -8017,7 +8023,7 @@
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -8033,7 +8039,7 @@
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -8058,23 +8064,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F5FFE7-3E5A-4739-98E5-B51767290A45}">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C21" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="40" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.15625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.26171875" customWidth="1"/>
+    <col min="6" max="6" width="19.26171875" customWidth="1"/>
+    <col min="7" max="7" width="11.41796875" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -8082,7 +8088,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
@@ -8093,7 +8099,7 @@
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
     </row>
-    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
@@ -8101,25 +8107,25 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="14"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="20"/>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="20"/>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="21"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="24" t="s">
         <v>16</v>
       </c>
@@ -8163,7 +8169,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="38" t="s">
         <v>207</v>
       </c>
@@ -8195,7 +8201,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="38"/>
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
@@ -8211,7 +8217,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="38"/>
       <c r="B11" s="27" t="s">
         <v>193</v>
@@ -8233,13 +8239,15 @@
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="10"/>
+      <c r="J11" s="42" t="s">
+        <v>258</v>
+      </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="38"/>
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
@@ -8255,7 +8263,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="38"/>
       <c r="B13" s="27" t="s">
         <v>194</v>
@@ -8285,7 +8293,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="38"/>
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
@@ -8301,7 +8309,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="38"/>
       <c r="B15" s="27" t="s">
         <v>196</v>
@@ -8331,7 +8339,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="38"/>
       <c r="B16" s="27"/>
       <c r="C16" s="27"/>
@@ -8347,7 +8355,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="38"/>
       <c r="B17" s="27" t="s">
         <v>198</v>
@@ -8359,19 +8367,21 @@
         <v>364</v>
       </c>
       <c r="E17" s="7"/>
-      <c r="F17" s="11"/>
+      <c r="F17" s="43"/>
       <c r="G17" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="10"/>
+      <c r="J17" s="42" t="s">
+        <v>258</v>
+      </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="38"/>
       <c r="B18" s="27"/>
       <c r="C18" s="27"/>
@@ -8387,7 +8397,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="38"/>
       <c r="B19" s="27" t="s">
         <v>200</v>
@@ -8417,7 +8427,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="38"/>
       <c r="B20" s="27"/>
       <c r="C20" s="27"/>
@@ -8433,7 +8443,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="38"/>
       <c r="B21" s="27" t="s">
         <v>202</v>
@@ -8463,7 +8473,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="38"/>
       <c r="B22" s="27"/>
       <c r="C22" s="27"/>
@@ -8489,7 +8499,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="38"/>
       <c r="B23" s="27" t="s">
         <v>204</v>
@@ -8519,7 +8529,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="38"/>
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
@@ -8535,7 +8545,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="38"/>
       <c r="B25" s="27" t="s">
         <v>206</v>
@@ -8557,13 +8567,15 @@
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="10"/>
+      <c r="J25" s="42" t="s">
+        <v>30</v>
+      </c>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="37"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -8579,7 +8591,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="30"/>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
@@ -8595,7 +8607,7 @@
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="30"/>
       <c r="B28" s="35"/>
       <c r="C28" s="23"/>
@@ -8611,7 +8623,7 @@
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="30"/>
       <c r="B29" s="27"/>
       <c r="C29" s="31"/>
@@ -8627,7 +8639,7 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="30"/>
       <c r="B30" s="26"/>
       <c r="C30" s="23"/>
@@ -8643,7 +8655,7 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="30"/>
       <c r="B31" s="26"/>
       <c r="C31" s="32"/>
@@ -8659,7 +8671,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="30"/>
       <c r="B32" s="26"/>
       <c r="C32" s="23"/>
@@ -8675,7 +8687,7 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="30"/>
       <c r="B33" s="26"/>
       <c r="C33" s="31"/>
@@ -8691,7 +8703,7 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="30"/>
       <c r="B34" s="26"/>
       <c r="C34" s="23"/>
@@ -8707,7 +8719,7 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="30"/>
       <c r="B35" s="26"/>
       <c r="C35" s="32"/>
@@ -8723,7 +8735,7 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="30"/>
       <c r="B36" s="26"/>
       <c r="C36" s="23"/>
@@ -8739,7 +8751,7 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="30"/>
       <c r="B37" s="26"/>
       <c r="C37" s="33"/>
@@ -8755,7 +8767,7 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="30"/>
       <c r="B38" s="26"/>
       <c r="C38" s="23"/>
@@ -8771,7 +8783,7 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="30"/>
       <c r="B39" s="26"/>
       <c r="C39" s="32"/>
@@ -8787,7 +8799,7 @@
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="30"/>
       <c r="B40" s="26"/>
       <c r="C40" s="23"/>
@@ -8803,7 +8815,7 @@
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2"/>
       <c r="B41" s="34"/>
       <c r="C41" s="2"/>
@@ -8819,7 +8831,7 @@
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2"/>
       <c r="B42" s="26"/>
       <c r="C42" s="28"/>
@@ -8835,7 +8847,7 @@
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2"/>
       <c r="B43" s="26"/>
       <c r="C43" s="29"/>
@@ -8851,7 +8863,7 @@
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2"/>
       <c r="B44" s="26"/>
       <c r="C44" s="23"/>
@@ -8867,7 +8879,7 @@
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2"/>
       <c r="B45" s="26"/>
       <c r="C45" s="7"/>
@@ -8883,7 +8895,7 @@
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2"/>
       <c r="B46" s="26"/>
       <c r="C46" s="23"/>
@@ -8899,7 +8911,7 @@
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2"/>
       <c r="B47" s="26"/>
       <c r="C47" s="7"/>
@@ -8915,7 +8927,7 @@
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="2"/>
       <c r="B48" s="26"/>
       <c r="C48" s="23"/>
@@ -8931,7 +8943,7 @@
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="7"/>
@@ -8947,7 +8959,7 @@
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -8963,7 +8975,7 @@
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -8979,7 +8991,7 @@
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="7"/>
@@ -8995,7 +9007,7 @@
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -9011,7 +9023,7 @@
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -9027,7 +9039,7 @@
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="7"/>
@@ -9043,7 +9055,7 @@
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -9059,7 +9071,7 @@
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -9075,7 +9087,7 @@
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="7"/>
@@ -9091,7 +9103,7 @@
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="7"/>
@@ -9107,7 +9119,7 @@
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -9123,7 +9135,7 @@
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -9139,7 +9151,7 @@
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -9155,7 +9167,7 @@
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -9171,7 +9183,7 @@
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -9187,7 +9199,7 @@
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -9203,7 +9215,7 @@
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -9219,7 +9231,7 @@
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -9235,7 +9247,7 @@
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>

</xml_diff>